<commit_message>
Add Responsibility Pattern, Command Pattern
</commit_message>
<xml_diff>
--- a/Design Pattern Start.xlsx
+++ b/Design Pattern Start.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Desktop\GoF blog\ch01 Start\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\github\GoF_CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48B9887-D352-4658-8042-473016C0D118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAED4AB-1658-4F48-92D9-2567CC79012C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="设计原则" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>创建型模式</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,7 +248,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -259,7 +259,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -277,7 +277,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -288,7 +288,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -306,7 +306,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -317,7 +317,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -335,7 +335,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -346,7 +346,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -364,7 +364,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -375,7 +375,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -393,7 +393,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -404,7 +404,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -422,7 +422,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -433,7 +433,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -496,7 +496,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -507,16 +507,12 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>，是一类最常见的设计模式，在软件开发中应用非常广泛。创建型模式描述如何将对象的创建和使用分离，让用户在使用对象时无需关心对象的创建细节，从而降低系统的耦合度，让设计方案更易于修改和扩展。每一个创建型模式都通过采用不同的解决方案来回答3个问题：What-创建什么，Who-由谁创建， When-何时创建</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>描述类或对象如何交互和怎样分配职责</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -534,11 +530,6 @@
   <si>
     <t>非GoF23模式之一，
 是其他工厂模式的基础</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>处理类或对象的组合
-结构型模式关注如何将现有类或对象组织在一起形成更加强大的结构。不同不结构型模式从不同的角度组合类或对象。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -661,7 +652,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -672,7 +663,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -684,7 +675,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -695,7 +686,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -707,7 +698,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -718,7 +709,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -730,7 +721,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -751,7 +742,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -762,7 +753,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -773,7 +764,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -784,7 +775,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -803,7 +794,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -814,7 +805,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -830,7 +821,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -841,7 +832,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -851,7 +842,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -862,7 +853,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -881,7 +872,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -892,7 +883,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -904,7 +895,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -915,7 +906,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -934,7 +925,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -945,7 +936,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -957,7 +948,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -968,7 +959,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -978,7 +969,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -1028,22 +1019,125 @@
 智能引用代理(Smart Reference Proxy)：当一个对象被引用时，提供一些额外的操作，例如将对象被调用的次数记录下来。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t>处理类或对象的</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>组合</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+结构型模式关注如何将现有类或对象组织在一起形成更加强大的结构。不同不结构型模式从不同的角度组合类或对象。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>描述类或对象如何</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>交互</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>和怎样</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>分配职责</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+关注系统中类或对象之间的交互，研究系统在运行时对象之间的相互通信与协作，进一步明确对象的职责。
+类行为型模式：使用继承关系在几个类之间分配行为，主要通过多态等方式来分配父类和子类的职责；
+对象行为型模式：使用对象的关联关系来分配行为，主要通过对象关联等方式来分配两个或多个类的职责</t>
+    </r>
+  </si>
+  <si>
+    <t>职责链模式
+(Chain of Responsibility)</t>
+  </si>
+  <si>
+    <t>避免将一个请求的发送者与接收者耦合在一起，让多个对象都有机会处理请求。将接收请求的对象连接成一条链，并且沿着这条链传递请求，直到有一个对象能够处理它为止
+Avoid coupling the sender of a request to its receiver by giving more than one object a chance to handle the request. Chain the receiving objects and pass the request along the chain until an object handles it.</t>
+  </si>
+  <si>
+    <t>命令模式
+(Command)</t>
+  </si>
+  <si>
+    <t>将一个请求封装为一个对象，从而让你可以用不同的请求对客户进行参数化，对请求排队或者记录请求日志，以及支持可撤销的操作
+Encapsulate a request as an object, thereby letting you parameterize clients with different requests, queue or log requests, and support undoable operations.</t>
+  </si>
+  <si>
+    <t>又叫责任链模式
+对象行为型模式</t>
+  </si>
+  <si>
+    <t>又叫动作模式(Action)或事务模式(Transaction)
+对象行为型模式
+实现命令队列，记录请求日志，撤销操作
+宏命令(Macro Command)又称为组合命令(Composite Command)，是组合模式和命令模联用的产物</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1052,7 +1146,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1060,7 +1154,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1069,13 +1163,21 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1118,6 +1220,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -1427,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1496,9 +1604,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1532,6 +1637,18 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1568,9 +1685,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1854,13 +1972,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="63.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="63.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
@@ -1871,7 +1989,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="60">
       <c r="A2" s="22" t="s">
         <v>40</v>
       </c>
@@ -1882,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45">
       <c r="A3" s="22" t="s">
         <v>41</v>
       </c>
@@ -1893,7 +2011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="45">
       <c r="A4" s="22" t="s">
         <v>42</v>
       </c>
@@ -1904,7 +2022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="69" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="75">
       <c r="A5" s="22" t="s">
         <v>43</v>
       </c>
@@ -1915,7 +2033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="60">
       <c r="A6" s="22" t="s">
         <v>44</v>
       </c>
@@ -1926,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="45">
       <c r="A7" s="22" t="s">
         <v>45</v>
       </c>
@@ -1937,7 +2055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="60.75" thickBot="1">
       <c r="A8" s="24" t="s">
         <v>46</v>
       </c>
@@ -1959,33 +2077,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="73.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="73.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="48"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="51"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="53"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -1996,8 +2114,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2010,16 +2128,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="44"/>
+    <row r="4" spans="1:6">
+      <c r="A4" s="47"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2032,8 +2150,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
+    <row r="6" spans="1:6">
+      <c r="A6" s="47"/>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
@@ -2044,8 +2162,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
+    <row r="7" spans="1:6">
+      <c r="A7" s="47"/>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
@@ -2056,8 +2174,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="44"/>
+    <row r="8" spans="1:6">
+      <c r="A8" s="47"/>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
@@ -2068,8 +2186,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
+    <row r="9" spans="1:6">
+      <c r="A9" s="47"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -2078,8 +2196,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
+    <row r="10" spans="1:6">
+      <c r="A10" s="47"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -2088,8 +2206,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
+    <row r="11" spans="1:6">
+      <c r="A11" s="47"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>19</v>
@@ -2098,24 +2216,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="47"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A13" s="48"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="15" spans="1:6" ht="45">
       <c r="E15" s="8" t="s">
         <v>61</v>
       </c>
@@ -2123,7 +2241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="60">
       <c r="E16" s="10" t="s">
         <v>62</v>
       </c>
@@ -2131,7 +2249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="5:7" ht="69" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7" ht="75">
       <c r="E17" s="10" t="s">
         <v>63</v>
       </c>
@@ -2140,36 +2258,36 @@
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="5:7" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7" ht="45">
       <c r="E18" s="10" t="s">
         <v>64</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" ht="27.6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" ht="105">
       <c r="E19" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F19" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" ht="60">
+      <c r="E20" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="5:7" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" ht="75.75" thickBot="1">
+      <c r="E21" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="13" t="s">
-        <v>69</v>
-      </c>
       <c r="F21" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2187,23 +2305,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76C8911-8254-4ED9-A36C-74122DF5E80A}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" customWidth="1"/>
-    <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="66.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="66.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="22.15" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>29</v>
       </c>
@@ -2220,12 +2338,12 @@
         <v>39</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>87</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="54" t="s">
+        <v>85</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>58</v>
@@ -2239,17 +2357,17 @@
       <c r="E2" s="27">
         <v>3</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+      <c r="F2" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60">
+      <c r="A3" s="55"/>
       <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -2257,17 +2375,17 @@
       <c r="E3" s="27">
         <v>5</v>
       </c>
-      <c r="F3" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="F3" s="37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60">
+      <c r="A4" s="55"/>
       <c r="B4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="5">
         <v>4</v>
@@ -2275,17 +2393,17 @@
       <c r="E4" s="27">
         <v>5</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="F4" s="39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60">
+      <c r="A5" s="55"/>
       <c r="B5" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D5" s="5">
         <v>4</v>
@@ -2293,17 +2411,17 @@
       <c r="E5" s="27">
         <v>2</v>
       </c>
-      <c r="F5" s="40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+      <c r="F5" s="39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60">
+      <c r="A6" s="55"/>
       <c r="B6" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="5">
         <v>3</v>
@@ -2311,159 +2429,192 @@
       <c r="E6" s="27">
         <v>3</v>
       </c>
-      <c r="F6" s="38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="69" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="33" t="s">
+      <c r="F6" s="37" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75">
+      <c r="A7" s="55"/>
+      <c r="B7" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="34">
+        <v>4</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="120">
+      <c r="A8" s="56" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="36">
+        <v>2</v>
+      </c>
+      <c r="E8" s="36">
+        <v>4</v>
+      </c>
+      <c r="F8" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="34">
+    </row>
+    <row r="9" spans="1:6" ht="75">
+      <c r="A9" s="57"/>
+      <c r="B9" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D9" s="36">
+        <v>3</v>
+      </c>
+      <c r="E9" s="36">
+        <v>3</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="90">
+      <c r="A10" s="57"/>
+      <c r="B10" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="36">
+        <v>3</v>
+      </c>
+      <c r="E10" s="36">
+        <v>4</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="60">
+      <c r="A11" s="57"/>
+      <c r="B11" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="36">
+        <v>3</v>
+      </c>
+      <c r="E11" s="36">
+        <v>3</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60">
+      <c r="A12" s="57"/>
+      <c r="B12" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="36">
         <v>1</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E12" s="36">
+        <v>5</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="150">
+      <c r="A13" s="57"/>
+      <c r="B13" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="36">
         <v>4</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="37">
+      <c r="E13" s="36">
+        <v>1</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="315">
+      <c r="A14" s="58"/>
+      <c r="B14" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="36">
+        <v>3</v>
+      </c>
+      <c r="E14" s="36">
+        <v>4</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="90">
+      <c r="A15" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="45">
+        <v>3</v>
+      </c>
+      <c r="E15" s="45">
         <v>2</v>
       </c>
-      <c r="E8" s="37">
+      <c r="F15" s="46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75">
+      <c r="A16" s="59"/>
+      <c r="B16" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="45">
+        <v>3</v>
+      </c>
+      <c r="E16" s="45">
         <v>4</v>
       </c>
-      <c r="F8" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="37">
-        <v>3</v>
-      </c>
-      <c r="E9" s="37">
-        <v>3</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
-      <c r="B10" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="37">
-        <v>3</v>
-      </c>
-      <c r="E10" s="37">
-        <v>4</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="54"/>
-      <c r="B11" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="37">
-        <v>3</v>
-      </c>
-      <c r="E11" s="37">
-        <v>3</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="54"/>
-      <c r="B12" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="37">
-        <v>1</v>
-      </c>
-      <c r="E12" s="37">
-        <v>5</v>
-      </c>
-      <c r="F12" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="110.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="54"/>
-      <c r="B13" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="37">
-        <v>4</v>
-      </c>
-      <c r="E13" s="37">
-        <v>1</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="220.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="37">
-        <v>3</v>
-      </c>
-      <c r="E14" s="37">
-        <v>4</v>
-      </c>
-      <c r="F14" s="41" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="32" t="s">
-        <v>86</v>
+      <c r="F16" s="46" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Template Method Pattern
</commit_message>
<xml_diff>
--- a/Design Pattern Start.xlsx
+++ b/Design Pattern Start.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\dotnet\GoF_CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C0A47A-C5BA-4472-88DF-ED8979E44DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3A1C9E-6F0B-47C9-A9C2-3A69B946FDC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="140">
   <si>
     <t>创建型模式</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1295,6 +1295,16 @@
   <si>
     <t>开闭原则，单一职责原则
 又叫政策(Policy)模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定义一个操作中算法的框架，而将一些步骤延迟到子类中。模板方法模式使得子类不改变一个算法的结构即可重定义该算法的某些特定步骤。
+Define the skeleton of an algorithm in an operation, deferring some steps to subclasses. Template method lets subclasses redefine certain steps of an algorithm without changing the algorithm's structure.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开闭原则
+模板方法，是在抽象类中定义，把基本操作方法(Primitive Operation)组合形成一个总算法或一个总行为得方法。子类不会修改它，只会修改基本方法。由于模板方法是具体方法，所以模板方法模式得抽象层是抽象类，而不是接口。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2499,7 +2509,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -2935,19 +2945,23 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="76.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="60"/>
       <c r="B24" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="39"/>
+      <c r="C24" s="39" t="s">
+        <v>138</v>
+      </c>
       <c r="D24" s="40">
         <v>2</v>
       </c>
       <c r="E24" s="40">
         <v>3</v>
       </c>
-      <c r="F24" s="39"/>
+      <c r="F24" s="39" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="61"/>

</xml_diff>